<commit_message>
updated on 26 Mar 2018
</commit_message>
<xml_diff>
--- a/cucumber-java-template/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
+++ b/cucumber-java-template/src/test/resources/ExcelFiles/AutomationControlSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raghav Pal\Desktop\Desktop\Projects\Projects\cucumber-jvm-template-master 2.0\src\test\resources\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raghav Pal\git\TXAutomate\cucumber-java-template\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t>N</t>
   </si>
@@ -228,61 +228,70 @@
     <t>UDID</t>
   </si>
   <si>
-    <t>Damcotest@gmail.com</t>
+    <t>Build_1.0</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://testingxpert.atlassian.net</t>
+  </si>
+  <si>
+    <t>Automation Demo</t>
+  </si>
+  <si>
+    <t>10001</t>
+  </si>
+  <si>
+    <t>0001505811674768-242ac112-0001</t>
+  </si>
+  <si>
+    <t>https://uat-upcenhancements.hostedinsurance.com/AgentPortal/login</t>
+  </si>
+  <si>
+    <t>testingxperts11@gmail.com</t>
+  </si>
+  <si>
+    <t>Damco@123</t>
+  </si>
+  <si>
+    <t>04f4865d006bb877</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>Nexus 5</t>
+  </si>
+  <si>
+    <t>raghavpal1</t>
+  </si>
+  <si>
+    <t>2LV2zzTV8NpH2ZRi57fE</t>
+  </si>
+  <si>
+    <t>raghav.pal@testingxperts.com</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>VitaminShoppe</t>
+  </si>
+  <si>
+    <t>https://redesign.perf.vitaminshoppe.com/</t>
   </si>
   <si>
     <t>Project Name</t>
   </si>
   <si>
-    <t>Build_1.0</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>https://testingxpert.atlassian.net</t>
-  </si>
-  <si>
-    <t>Automation Demo</t>
-  </si>
-  <si>
-    <t>10001</t>
-  </si>
-  <si>
-    <t>0001505811674768-242ac112-0001</t>
+    <t>WINDOWS_10</t>
   </si>
   <si>
     <t>Local</t>
   </si>
   <si>
-    <t>https://uat-upcenhancements.hostedinsurance.com/AgentPortal/login</t>
-  </si>
-  <si>
-    <t>CHROME</t>
-  </si>
-  <si>
-    <t>testingxperts11@gmail.com</t>
-  </si>
-  <si>
-    <t>Damco@123</t>
-  </si>
-  <si>
-    <t>04f4865d006bb877</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>Nexus 5</t>
-  </si>
-  <si>
-    <t>raghavpal1</t>
-  </si>
-  <si>
-    <t>2LV2zzTV8NpH2ZRi57fE</t>
-  </si>
-  <si>
-    <t>MAC_Yosemite</t>
+    <t>FIREFOX</t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -409,6 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,7 +427,14 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -826,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:B55"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -842,20 +859,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -888,7 +905,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -898,8 +915,8 @@
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>73</v>
+      <c r="B6" s="15" t="s">
+        <v>70</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -921,7 +938,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -945,7 +962,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="3"/>
@@ -956,7 +973,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="3"/>
@@ -966,8 +983,8 @@
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
-        <v>82</v>
+      <c r="B12" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="3"/>
@@ -978,7 +995,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="3"/>
@@ -1001,8 +1018,8 @@
       <c r="A15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
-        <v>64</v>
+      <c r="B15" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1167,7 +1184,7 @@
         <v>54</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1178,7 +1195,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1189,7 +1206,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -1240,7 +1257,7 @@
         <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1251,7 +1268,7 @@
         <v>53</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1270,7 +1287,7 @@
       <c r="A40" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C40" s="3"/>
@@ -1305,7 +1322,7 @@
         <v>58</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -1316,7 +1333,7 @@
         <v>59</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -1327,7 +1344,7 @@
         <v>60</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -1372,7 +1389,7 @@
         <v>58</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -1383,7 +1400,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -1394,7 +1411,7 @@
         <v>63</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -1430,43 +1447,48 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:E9 A10:A12 C10:E12 B9:B11">
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="8" priority="14">
       <formula>$B$8="Local"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="expression" dxfId="6" priority="11">
+    <cfRule type="expression" dxfId="7" priority="12">
       <formula>$B$29="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="expression" dxfId="5" priority="10">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>$B$22="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:B26">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>$B$21="JIRA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36 B38">
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$B$21&lt;&gt;"JIRA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>$B$36="NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$B$21&lt;&gt;"JIRA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B$29="NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$B$29="NO"</formula>
+      <formula>$B$8="Local"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
@@ -1496,16 +1518,18 @@
     <hyperlink ref="B30" r:id="rId1"/>
     <hyperlink ref="B31" r:id="rId2"/>
     <hyperlink ref="B32" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B15" r:id="rId4"/>
+    <hyperlink ref="B40" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E7"/>
+  <dimension ref="B3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -1517,7 +1541,7 @@
     <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>42</v>
       </c>
@@ -1525,7 +1549,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
@@ -1533,7 +1557,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
@@ -1541,7 +1565,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
@@ -1549,7 +1573,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1557,7 +1581,27 @@
         <v>48</v>
       </c>
     </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C12" r:id="rId1"/>
+    <hyperlink ref="C13" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>